<commit_message>
New test classes HomeTest and DataStructure added.
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testData/testdata.xlsx
+++ b/src/test/java/resources/testData/testdata.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\DsalgoTestNg\src\test\resources\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655F54B0-EA35-4F09-9302-A3674CC63616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8B6AC770-B02F-47DD-9F35-DCF95CF2C00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10060" activeTab="3" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +14,7 @@
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:P13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -578,7 +574,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -772,7 +768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D3829F-7C9E-4A7F-8E08-32F4F2BF4D32}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>